<commit_message>
finished parser for local data
</commit_message>
<xml_diff>
--- a/parser/Movie Data.xlsx
+++ b/parser/Movie Data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/irmakozer/Dropbox/My Mac (Irmak’s MacBook Pro)/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sinanozer/Documents/GitHub/movie-data/parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB889F8-8F03-D34F-B0B8-B5F67EA0588B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFEB617-2BEC-6541-A91A-7DA9EE84F692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{C9D72D0A-8A7E-E14A-8162-618F63719EB7}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="15760" activeTab="1" xr2:uid="{C9D72D0A-8A7E-E14A-8162-618F63719EB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="CSV Export" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="names_dates_1" localSheetId="0">Sheet2!$A$2:$M$376</definedName>
@@ -39,7 +40,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{A3E48783-7F08-5F4C-B26B-42356C8D6849}" name="names_dates1" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/irmakozer/Dropbox/My Mac (Irmak’s MacBook Pro)/Desktop/names_dates.txt" decimal="," thousands="." tab="0" space="1" consecutive="1">
+    <textPr sourceFile="/Users/irmakozer/Dropbox/My Mac (Irmak’s MacBook Pro)/Desktop/names_dates.txt" decimal="," thousands="." tab="0" space="1" consecutive="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="230">
   <si>
     <t>---</t>
   </si>
@@ -750,7 +751,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -803,21 +804,21 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1143,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9743E0AA-56AB-0541-AD1D-0B05E77F7572}">
   <dimension ref="A1:E376"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A345" sqref="A345:XFD345"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5506,4 +5507,449 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E69DE43-3042-CA4F-8355-F15933D3F9A6}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3">
+        <v>44197</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>44198</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>44199</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>44200</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>44201</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>44202</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>44203</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>44204</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>44205</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>44206</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>44207</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>44208</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>44209</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>44210</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>44211</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>44212</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>44213</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>44214</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>44215</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>44216</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>44217</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>44218</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>44219</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>44220</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>44221</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>44222</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>44223</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>44224</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>44225</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>44226</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>44227</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>